<commit_message>
consideration of userbility questionnaire
</commit_message>
<xml_diff>
--- a/literature/04.reseach-interface-comparative-experiments/実験分析入力実験.xlsx
+++ b/literature/04.reseach-interface-comparative-experiments/実験分析入力実験.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="主観" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="67">
   <si>
     <t>操作のわかりやすさ</t>
   </si>
@@ -78,13 +78,6 @@
     <t>検定</t>
     <rPh sb="0" eb="2">
       <t>ケン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>有意差あり</t>
-    <rPh sb="0" eb="3">
-      <t>ユウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -388,12 +381,23 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>T検定</t>
+    <rPh sb="1" eb="3">
+      <t>ケン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>見やすさ</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -447,6 +451,14 @@
       <sz val="12"/>
       <color theme="5"/>
       <name val="ＭＳ Ｐゴシック"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
@@ -590,7 +602,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="179">
+  <cellStyleXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -770,8 +782,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -814,8 +828,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="179">
+  <cellStyles count="181">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -905,6 +920,7 @@
     <cellStyle name="ハイパーリンク" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -995,6 +1011,7 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="180" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1105,7 +1122,7 @@
                   <c:v>構成のわかりやすさ</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>見易さ</c:v>
+                  <c:v>見やすさ</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>反応のよさ</c:v>
@@ -1218,7 +1235,7 @@
                   <c:v>構成のわかりやすさ</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>見易さ</c:v>
+                  <c:v>見やすさ</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>反応のよさ</c:v>
@@ -1257,11 +1274,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2119804152"/>
-        <c:axId val="-2125086280"/>
+        <c:axId val="2072215160"/>
+        <c:axId val="2072211544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2119804152"/>
+        <c:axId val="2072215160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1280,7 +1297,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125086280"/>
+        <c:crossAx val="2072211544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1288,7 +1305,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2125086280"/>
+        <c:axId val="2072211544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1328,7 +1345,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2119804152"/>
+        <c:crossAx val="2072215160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1532,11 +1549,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2036743000"/>
-        <c:axId val="2083289848"/>
+        <c:axId val="2107876392"/>
+        <c:axId val="2107865800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2036743000"/>
+        <c:axId val="2107876392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1581,7 +1598,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083289848"/>
+        <c:crossAx val="2107865800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1589,7 +1606,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2083289848"/>
+        <c:axId val="2107865800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.0"/>
@@ -1649,7 +1666,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2036743000"/>
+        <c:crossAx val="2107876392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
@@ -1778,8 +1795,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2101290056"/>
-        <c:axId val="-2129380584"/>
+        <c:axId val="2107790424"/>
+        <c:axId val="2107785352"/>
       </c:barChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1835,11 +1852,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2121828344"/>
-        <c:axId val="-2127444248"/>
+        <c:axId val="2107773720"/>
+        <c:axId val="2107779256"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="2101290056"/>
+        <c:axId val="2107790424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1861,7 +1878,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
@@ -1877,7 +1893,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2129380584"/>
+        <c:crossAx val="2107785352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1885,7 +1901,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129380584"/>
+        <c:axId val="2107785352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1920,7 +1936,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0.0_);[Red]\(#,##0.0\)" sourceLinked="0"/>
@@ -1937,13 +1952,13 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2101290056"/>
+        <c:crossAx val="2107790424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2127444248"/>
+        <c:axId val="2107779256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1989,12 +2004,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2121828344"/>
+        <c:crossAx val="2107773720"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2121828344"/>
+        <c:axId val="2107773720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2003,7 +2018,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127444248"/>
+        <c:crossAx val="2107779256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2166,8 +2181,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-60"/>
-        <c:axId val="-2128491144"/>
-        <c:axId val="2118487832"/>
+        <c:axId val="2107735432"/>
+        <c:axId val="2107729736"/>
       </c:barChart>
       <c:barChart>
         <c:barDir val="col"/>
@@ -2295,11 +2310,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2120325976"/>
-        <c:axId val="2120802456"/>
+        <c:axId val="2107718312"/>
+        <c:axId val="2107724264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2128491144"/>
+        <c:axId val="2107735432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2344,7 +2359,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2118487832"/>
+        <c:crossAx val="2107729736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2352,7 +2367,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2118487832"/>
+        <c:axId val="2107729736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2374,7 +2389,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2391,12 +2405,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2128491144"/>
+        <c:crossAx val="2107735432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2120802456"/>
+        <c:axId val="2107724264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.0"/>
@@ -2432,7 +2446,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0.0_);[Red]\(#,##0.0\)" sourceLinked="0"/>
@@ -2449,13 +2462,13 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2120325976"/>
+        <c:crossAx val="2107718312"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2120325976"/>
+        <c:axId val="2107718312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2464,7 +2477,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2120802456"/>
+        <c:crossAx val="2107724264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2482,7 +2495,6 @@
         <c:idx val="2"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -2642,11 +2654,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2118271928"/>
-        <c:axId val="2118265864"/>
+        <c:axId val="2107692456"/>
+        <c:axId val="2107689432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2118271928"/>
+        <c:axId val="2107692456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2665,7 +2677,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2118265864"/>
+        <c:crossAx val="2107689432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2673,7 +2685,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2118265864"/>
+        <c:axId val="2107689432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2690,11 +2702,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="ja-JP" altLang="en-US" sz="1200"/>
-                  <a:t>一文字あたりの</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="ja-JP" altLang="en-US" sz="1200"/>
-                  <a:t>入力時間</a:t>
+                  <a:t>一文字あたりの入力時間</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" altLang="ja-JP" sz="1200"/>
@@ -2712,7 +2720,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2729,7 +2736,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2118271928"/>
+        <c:crossAx val="2107692456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2898,11 +2905,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2126189480"/>
-        <c:axId val="-2125674968"/>
+        <c:axId val="2107640600"/>
+        <c:axId val="2110112808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2126189480"/>
+        <c:axId val="2107640600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2921,7 +2928,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125674968"/>
+        <c:crossAx val="2110112808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2929,7 +2936,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2125674968"/>
+        <c:axId val="2110112808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2951,7 +2958,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2968,7 +2974,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2126189480"/>
+        <c:crossAx val="2107640600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3121,11 +3127,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2127198712"/>
-        <c:axId val="-2121731656"/>
+        <c:axId val="2110153256"/>
+        <c:axId val="2110158712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2127198712"/>
+        <c:axId val="2110153256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3170,7 +3176,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2121731656"/>
+        <c:crossAx val="2110158712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3178,7 +3184,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2121731656"/>
+        <c:axId val="2110158712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3237,7 +3243,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2127198712"/>
+        <c:crossAx val="2110153256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3463,11 +3469,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2121167912"/>
-        <c:axId val="-2126784248"/>
+        <c:axId val="2110195304"/>
+        <c:axId val="2110198184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2121167912"/>
+        <c:axId val="2110195304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3486,7 +3492,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2126784248"/>
+        <c:crossAx val="2110198184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3494,7 +3500,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2126784248"/>
+        <c:axId val="2110198184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3516,6 +3522,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3532,13 +3539,14 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2121167912"/>
+        <c:crossAx val="2110195304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -3715,11 +3723,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2046405832"/>
-        <c:axId val="-2122197672"/>
+        <c:axId val="2062459096"/>
+        <c:axId val="2062462104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2046405832"/>
+        <c:axId val="2062459096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3738,7 +3746,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2122197672"/>
+        <c:crossAx val="2062462104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3746,7 +3754,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122197672"/>
+        <c:axId val="2062462104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3768,6 +3776,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3784,7 +3793,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2046405832"/>
+        <c:crossAx val="2062459096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3793,6 +3802,11 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -3812,9 +3826,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>927100</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4061,15 +4075,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
+      <xdr:colOff>698500</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4415,8 +4429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:L13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -4549,37 +4563,37 @@
       </c>
     </row>
     <row r="8" spans="3:12">
-      <c r="D8" t="s">
-        <v>12</v>
+      <c r="E8" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="3:12">
       <c r="C9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <f>TTEST(D3:F3, H3:J3, 2, 1)</f>
         <v>0.18350341907227463</v>
       </c>
       <c r="I9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" t="s">
+        <v>52</v>
+      </c>
+      <c r="K9" t="s">
         <v>51</v>
       </c>
-      <c r="J9" t="s">
-        <v>53</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>52</v>
-      </c>
-      <c r="L9" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="10" spans="3:12">
       <c r="C10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D10">
-        <f>TTEST(D4:F4, H4:J4, 2, 1)</f>
+      <c r="E10">
+        <f t="shared" ref="E10:E12" si="0">TTEST(D4:F4, H4:J4, 2, 1)</f>
         <v>0.31400565942996472</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -4606,12 +4620,9 @@
       <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D11">
-        <f>TTEST(D5:F5, H5:J5, 2, 1)</f>
+      <c r="E11" s="20">
+        <f t="shared" si="0"/>
         <v>9.8524570233256663E-3</v>
-      </c>
-      <c r="E11" t="s">
-        <v>13</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>1</v>
@@ -4629,7 +4640,7 @@
         <v>5.333333333333333</v>
       </c>
       <c r="L11">
-        <f t="shared" ref="L11:L13" si="0">STDEV(H4:J4)</f>
+        <f t="shared" ref="L11:L13" si="1">STDEV(H4:J4)</f>
         <v>0.33333333333333348</v>
       </c>
     </row>
@@ -4637,19 +4648,19 @@
       <c r="C12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D12">
-        <f>TTEST(D6:F6, H6:J6, 2, 1)</f>
+      <c r="E12">
+        <f t="shared" si="0"/>
         <v>0.22540333075851626</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="I12">
         <f>AVERAGE(D5:F5)</f>
         <v>6.1111111111111116</v>
       </c>
       <c r="J12">
-        <f t="shared" ref="J12:J13" si="1">STDEV(D5:F5)</f>
+        <f t="shared" ref="J12:J13" si="2">STDEV(D5:F5)</f>
         <v>0.7698003589194935</v>
       </c>
       <c r="K12">
@@ -4657,7 +4668,7 @@
         <v>5</v>
       </c>
       <c r="L12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.57735026918962584</v>
       </c>
     </row>
@@ -4666,11 +4677,11 @@
         <v>5</v>
       </c>
       <c r="I13">
-        <f t="shared" ref="I13" si="2">AVERAGE(D6:F6)</f>
+        <f t="shared" ref="I13" si="3">AVERAGE(D6:F6)</f>
         <v>6.666666666666667</v>
       </c>
       <c r="J13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.57735026918962584</v>
       </c>
       <c r="K13">
@@ -4678,7 +4689,7 @@
         <v>6.333333333333333</v>
       </c>
       <c r="L13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.33333333333333348</v>
       </c>
     </row>
@@ -4703,8 +4714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G6" workbookViewId="0">
-      <selection activeCell="V26" sqref="V26"/>
+    <sheetView topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -4747,7 +4758,7 @@
     </row>
     <row r="3" spans="3:13">
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>15.19</v>
@@ -4759,7 +4770,7 @@
         <v>10.188333333333334</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3">
         <v>15.905000000000001</v>
@@ -4773,7 +4784,7 @@
     </row>
     <row r="4" spans="3:13">
       <c r="C4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" s="13">
         <f>AVERAGE(D3:F3)</f>
@@ -4794,7 +4805,7 @@
     </row>
     <row r="5" spans="3:13">
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <f>TTEST(D3:F3, H3:J3, 2, 1)</f>
@@ -4807,22 +4818,22 @@
     </row>
     <row r="7" spans="3:13">
       <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>26</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>27</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>28</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>29</v>
-      </c>
-      <c r="J7" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="3:13">
@@ -4847,7 +4858,7 @@
     </row>
     <row r="9" spans="3:13">
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>0.69057356881046428</v>
@@ -4885,7 +4896,7 @@
     </row>
     <row r="10" spans="3:13">
       <c r="C10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" s="13">
         <f>AVERAGE(D9:F9)</f>
@@ -4906,7 +4917,7 @@
     </row>
     <row r="12" spans="3:13">
       <c r="C12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12">
         <f>TTEST(D9:F9, H9:J9, 2, 1)</f>
@@ -4915,33 +4926,33 @@
     </row>
     <row r="17" spans="1:14">
       <c r="D17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" t="s">
         <v>37</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>38</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>39</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>40</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>41</v>
       </c>
-      <c r="I17" t="s">
-        <v>42</v>
-      </c>
       <c r="K17" t="s">
+        <v>54</v>
+      </c>
+      <c r="L17" t="s">
         <v>55</v>
-      </c>
-      <c r="L17" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>2</v>
@@ -4949,12 +4960,12 @@
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
       <c r="G18" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K18">
         <v>0.5936466202325299</v>
@@ -4967,7 +4978,7 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>3</v>
@@ -4979,16 +4990,16 @@
         <v>7</v>
       </c>
       <c r="G19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="I19" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="I19" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="J19" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K19">
         <f>STDEV(D9:F9)</f>
@@ -5001,7 +5012,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="5">
         <v>21.5</v>
@@ -5024,19 +5035,19 @@
     </row>
     <row r="21" spans="1:14">
       <c r="D21" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
       <c r="G21" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H21" s="17"/>
       <c r="I21" s="18"/>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D22" s="15">
         <f>AVERAGE(D20:F20)</f>
@@ -5082,20 +5093,20 @@
         <v>1.3200336007160932E-2</v>
       </c>
       <c r="I28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="8:12">
       <c r="I35" t="s">
+        <v>48</v>
+      </c>
+      <c r="L35" t="s">
         <v>49</v>
-      </c>
-      <c r="L35" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="36" spans="8:12">
       <c r="H36" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I36" s="5">
         <v>21.5</v>
@@ -5106,7 +5117,7 @@
     </row>
     <row r="37" spans="8:12">
       <c r="H37" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I37" s="5">
         <v>17</v>
@@ -5117,7 +5128,7 @@
     </row>
     <row r="38" spans="8:12">
       <c r="H38" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I38" s="5">
         <v>18.333333333333332</v>
@@ -5128,7 +5139,7 @@
     </row>
     <row r="39" spans="8:12">
       <c r="H39" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I39" s="5">
         <v>13.4</v>
@@ -5139,7 +5150,7 @@
     </row>
     <row r="40" spans="8:12">
       <c r="H40" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I40" s="5">
         <v>12.75</v>
@@ -5150,7 +5161,7 @@
     </row>
     <row r="41" spans="8:12">
       <c r="H41" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I41" s="5">
         <v>10.636363636363637</v>
@@ -5244,7 +5255,7 @@
         <v>1.3200336007160932E-2</v>
       </c>
       <c r="K3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="2:11">
@@ -5269,12 +5280,12 @@
     </row>
     <row r="5" spans="2:11">
       <c r="B5" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
       <c r="F5" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
@@ -5296,15 +5307,15 @@
     <row r="9" spans="2:11">
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="2:11">
       <c r="B10" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="5">
         <v>18.944444444444443</v>
@@ -5315,7 +5326,7 @@
     </row>
     <row r="11" spans="2:11">
       <c r="B11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="5">
         <f>STDEV(B4:D4)</f>
@@ -5351,8 +5362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H19"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A20" sqref="A19:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -5411,7 +5422,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="13">
         <f>AVERAGE(B4:D4)</f>
@@ -5434,22 +5445,22 @@
     </row>
     <row r="12" spans="1:8">
       <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
         <v>31</v>
       </c>
-      <c r="C12" t="s">
-        <v>32</v>
-      </c>
       <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
         <v>27</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>28</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>29</v>
-      </c>
-      <c r="G12" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -5485,15 +5496,15 @@
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="2:6">
       <c r="D18" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E18" s="5">
         <v>4.666666666666667</v>
@@ -5504,7 +5515,7 @@
     </row>
     <row r="19" spans="2:6">
       <c r="D19" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E19" s="5">
         <f>STDEV(B4:D4)</f>
@@ -5569,7 +5580,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>197</v>
@@ -5592,7 +5603,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>15.19</v>

</xml_diff>